<commit_message>
Removed zero shell wt and enforced some harvest dates
</commit_message>
<xml_diff>
--- a/Tests/Validation/Mungbean/ObservedData.xlsx
+++ b/Tests/Validation/Mungbean/ObservedData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Tests\Validation\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5D3E26-B3F9-4FE9-ABF7-5F44C7D306BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F19007-447D-45FA-9575-D22BA14F6E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11626" activeTab="1" xr2:uid="{9FA297CA-29B6-4A83-B4E5-4BA784BC781A}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11626" xr2:uid="{9FA297CA-29B6-4A83-B4E5-4BA784BC781A}"/>
   </bookViews>
   <sheets>
     <sheet name="PlantBiomassObserved" sheetId="1" r:id="rId1"/>
@@ -1190,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D7DBC0-8FFD-4004-98F0-2F6AD6B427E8}">
   <dimension ref="A1:W451"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="A203" sqref="A203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -4943,10 +4943,6 @@
       <c r="S199">
         <v>27.275245186799204</v>
       </c>
-      <c r="W199">
-        <f>V199-T199</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="200" spans="1:23">
       <c r="A200" t="s">
@@ -5118,10 +5114,6 @@
       </c>
       <c r="S203">
         <v>41.438129381846757</v>
-      </c>
-      <c r="W203">
-        <f>V203-T203</f>
-        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:23">
@@ -12393,7 +12385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DBEDAAD-4E07-4543-B9D3-A0ED902D4CED}">
   <dimension ref="A1:AC352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removing unreliable Branch Data and 0's from nodes
</commit_message>
<xml_diff>
--- a/Tests/Validation/Mungbean/ObservedData.xlsx
+++ b/Tests/Validation/Mungbean/ObservedData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pas075\Documents\ApsimX\Tests\Validation\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5302C1A7-D2A7-4E36-9195-CCAE8BB9337B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E5173A-B973-4F64-B98A-50B8093E17AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="4" xr2:uid="{9FA297CA-29B6-4A83-B4E5-4BA784BC781A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{9FA297CA-29B6-4A83-B4E5-4BA784BC781A}"/>
   </bookViews>
   <sheets>
     <sheet name="PlantBiomassObserved" sheetId="1" r:id="rId1"/>
@@ -33528,7 +33528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449093F9-5AE0-419F-A266-8D65D7DEDEE7}">
   <dimension ref="A1:L831"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -49089,8 +49089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BE5525-9C9B-4599-A191-AEACAF439893}">
   <dimension ref="A1:H831"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -53755,9 +53755,7 @@
         <v>35911</v>
       </c>
       <c r="D348" s="5"/>
-      <c r="E348" s="8">
-        <v>0</v>
-      </c>
+      <c r="E348" s="8"/>
       <c r="F348" s="8"/>
     </row>
     <row r="349" spans="1:6">
@@ -56690,9 +56688,6 @@
         <v>35964</v>
       </c>
       <c r="D569" s="5"/>
-      <c r="E569">
-        <v>0</v>
-      </c>
     </row>
     <row r="570" spans="1:6">
       <c r="A570" t="s">
@@ -58453,9 +58448,6 @@
       <c r="G700">
         <v>0.41457809879442498</v>
       </c>
-      <c r="H700">
-        <v>8.25</v>
-      </c>
     </row>
     <row r="701" spans="1:8">
       <c r="A701" t="s">
@@ -58487,9 +58479,6 @@
       <c r="G702">
         <v>0.52796780204857408</v>
       </c>
-      <c r="H702">
-        <v>8.4</v>
-      </c>
     </row>
     <row r="703" spans="1:8">
       <c r="A703" t="s">
@@ -58521,11 +58510,8 @@
       <c r="G704">
         <v>0.71239034243875055</v>
       </c>
-      <c r="H704">
-        <v>11.7</v>
-      </c>
-    </row>
-    <row r="705" spans="1:8">
+    </row>
+    <row r="705" spans="1:7">
       <c r="A705" t="s">
         <v>4</v>
       </c>
@@ -58536,7 +58522,7 @@
         <v>43908</v>
       </c>
     </row>
-    <row r="706" spans="1:8">
+    <row r="706" spans="1:7">
       <c r="A706" t="s">
         <v>4</v>
       </c>
@@ -58547,7 +58533,7 @@
         <v>43916</v>
       </c>
     </row>
-    <row r="707" spans="1:8">
+    <row r="707" spans="1:7">
       <c r="A707" t="s">
         <v>4</v>
       </c>
@@ -58566,11 +58552,8 @@
       <c r="G707">
         <v>0.44370598373247128</v>
       </c>
-      <c r="H707">
-        <v>12.049999999999999</v>
-      </c>
-    </row>
-    <row r="708" spans="1:8">
+    </row>
+    <row r="708" spans="1:7">
       <c r="A708" t="s">
         <v>4</v>
       </c>
@@ -58589,11 +58572,8 @@
       <c r="G708">
         <v>0.58040933831219732</v>
       </c>
-      <c r="H708">
-        <v>6.7499999999999991</v>
-      </c>
-    </row>
-    <row r="709" spans="1:8">
+    </row>
+    <row r="709" spans="1:7">
       <c r="A709" t="s">
         <v>4</v>
       </c>
@@ -58612,11 +58592,8 @@
       <c r="G709">
         <v>0.34910600109422335</v>
       </c>
-      <c r="H709">
-        <v>8.0500000000000007</v>
-      </c>
-    </row>
-    <row r="710" spans="1:8">
+    </row>
+    <row r="710" spans="1:7">
       <c r="A710" t="s">
         <v>4</v>
       </c>
@@ -58635,11 +58612,8 @@
       <c r="G710">
         <v>0.24874685927665507</v>
       </c>
-      <c r="H710">
-        <v>10.35</v>
-      </c>
-    </row>
-    <row r="711" spans="1:8">
+    </row>
+    <row r="711" spans="1:7">
       <c r="A711" t="s">
         <v>4</v>
       </c>
@@ -58658,11 +58632,8 @@
       <c r="G711">
         <v>0.50249378105604425</v>
       </c>
-      <c r="H711">
-        <v>11.100000000000001</v>
-      </c>
-    </row>
-    <row r="712" spans="1:8">
+    </row>
+    <row r="712" spans="1:7">
       <c r="A712" t="s">
         <v>4</v>
       </c>
@@ -58676,7 +58647,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="713" spans="1:8">
+    <row r="713" spans="1:7">
       <c r="A713" t="s">
         <v>4</v>
       </c>
@@ -58690,7 +58661,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="714" spans="1:8">
+    <row r="714" spans="1:7">
       <c r="A714" t="s">
         <v>4</v>
       </c>
@@ -58704,7 +58675,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="715" spans="1:8">
+    <row r="715" spans="1:7">
       <c r="A715" t="s">
         <v>4</v>
       </c>
@@ -58718,7 +58689,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="716" spans="1:8">
+    <row r="716" spans="1:7">
       <c r="A716" t="s">
         <v>4</v>
       </c>
@@ -58732,7 +58703,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="717" spans="1:8">
+    <row r="717" spans="1:7">
       <c r="A717" t="s">
         <v>4</v>
       </c>
@@ -58746,7 +58717,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="718" spans="1:8">
+    <row r="718" spans="1:7">
       <c r="A718" t="s">
         <v>4</v>
       </c>
@@ -58760,7 +58731,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="719" spans="1:8">
+    <row r="719" spans="1:7">
       <c r="A719" t="s">
         <v>4</v>
       </c>
@@ -58774,7 +58745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="720" spans="1:8">
+    <row r="720" spans="1:7">
       <c r="A720" t="s">
         <v>4</v>
       </c>
@@ -59236,7 +59207,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="753" spans="1:8">
+    <row r="753" spans="1:7">
       <c r="A753" t="s">
         <v>4</v>
       </c>
@@ -59250,7 +59221,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="754" spans="1:8">
+    <row r="754" spans="1:7">
       <c r="A754" t="s">
         <v>4</v>
       </c>
@@ -59264,7 +59235,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="755" spans="1:8">
+    <row r="755" spans="1:7">
       <c r="A755" t="s">
         <v>4</v>
       </c>
@@ -59278,7 +59249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="756" spans="1:8">
+    <row r="756" spans="1:7">
       <c r="A756" t="s">
         <v>4</v>
       </c>
@@ -59292,7 +59263,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="757" spans="1:8">
+    <row r="757" spans="1:7">
       <c r="A757" t="s">
         <v>4</v>
       </c>
@@ -59306,7 +59277,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="758" spans="1:8">
+    <row r="758" spans="1:7">
       <c r="A758" t="s">
         <v>4</v>
       </c>
@@ -59320,7 +59291,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="759" spans="1:8">
+    <row r="759" spans="1:7">
       <c r="A759" t="s">
         <v>4</v>
       </c>
@@ -59334,7 +59305,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="760" spans="1:8">
+    <row r="760" spans="1:7">
       <c r="A760" t="s">
         <v>4</v>
       </c>
@@ -59353,11 +59324,8 @@
       <c r="G760">
         <v>0.10897247358851676</v>
       </c>
-      <c r="H760">
-        <v>5.5500000000000007</v>
-      </c>
-    </row>
-    <row r="761" spans="1:8">
+    </row>
+    <row r="761" spans="1:7">
       <c r="A761" t="s">
         <v>4</v>
       </c>
@@ -59376,11 +59344,8 @@
       <c r="G761">
         <v>0.76852130744697178</v>
       </c>
-      <c r="H761">
-        <v>7.35</v>
-      </c>
-    </row>
-    <row r="762" spans="1:8">
+    </row>
+    <row r="762" spans="1:7">
       <c r="A762" t="s">
         <v>4</v>
       </c>
@@ -59394,7 +59359,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="763" spans="1:8">
+    <row r="763" spans="1:7">
       <c r="A763" t="s">
         <v>4</v>
       </c>
@@ -59408,7 +59373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="764" spans="1:8">
+    <row r="764" spans="1:7">
       <c r="A764" t="s">
         <v>4</v>
       </c>
@@ -59427,11 +59392,8 @@
       <c r="G764">
         <v>0.12247448713915883</v>
       </c>
-      <c r="H764">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="765" spans="1:8">
+    </row>
+    <row r="765" spans="1:7">
       <c r="A765" t="s">
         <v>4</v>
       </c>
@@ -59450,11 +59412,8 @@
       <c r="G765">
         <v>0.68328251843582888</v>
       </c>
-      <c r="H765">
-        <v>13.049999999999999</v>
-      </c>
-    </row>
-    <row r="766" spans="1:8">
+    </row>
+    <row r="766" spans="1:7">
       <c r="A766" t="s">
         <v>4</v>
       </c>
@@ -59468,7 +59427,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="767" spans="1:8">
+    <row r="767" spans="1:7">
       <c r="A767" t="s">
         <v>4</v>
       </c>
@@ -59482,7 +59441,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="768" spans="1:8">
+    <row r="768" spans="1:7">
       <c r="A768" t="s">
         <v>4</v>
       </c>
@@ -59501,11 +59460,8 @@
       <c r="G768">
         <v>0.25860201081971496</v>
       </c>
-      <c r="H768">
-        <v>5.15</v>
-      </c>
-    </row>
-    <row r="769" spans="1:8">
+    </row>
+    <row r="769" spans="1:7">
       <c r="A769" t="s">
         <v>4</v>
       </c>
@@ -59524,11 +59480,8 @@
       <c r="G769">
         <v>0.96136296475368743</v>
       </c>
-      <c r="H769">
-        <v>6.9249999999999998</v>
-      </c>
-    </row>
-    <row r="770" spans="1:8">
+    </row>
+    <row r="770" spans="1:7">
       <c r="A770" t="s">
         <v>4</v>
       </c>
@@ -59542,7 +59495,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="771" spans="1:8">
+    <row r="771" spans="1:7">
       <c r="A771" t="s">
         <v>4</v>
       </c>
@@ -59556,7 +59509,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="772" spans="1:8">
+    <row r="772" spans="1:7">
       <c r="A772" t="s">
         <v>4</v>
       </c>
@@ -59575,11 +59528,8 @@
       <c r="G772">
         <v>0.13479150566708564</v>
       </c>
-      <c r="H772">
-        <v>5.335</v>
-      </c>
-    </row>
-    <row r="773" spans="1:8">
+    </row>
+    <row r="773" spans="1:7">
       <c r="A773" t="s">
         <v>4</v>
       </c>
@@ -59598,11 +59548,8 @@
       <c r="G773">
         <v>0.91472331882378766</v>
       </c>
-      <c r="H773">
-        <v>7.9249999999999989</v>
-      </c>
-    </row>
-    <row r="774" spans="1:8">
+    </row>
+    <row r="774" spans="1:7">
       <c r="A774" t="s">
         <v>4</v>
       </c>
@@ -59616,7 +59563,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="775" spans="1:8">
+    <row r="775" spans="1:7">
       <c r="A775" t="s">
         <v>4</v>
       </c>
@@ -59630,7 +59577,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="776" spans="1:8">
+    <row r="776" spans="1:7">
       <c r="A776" t="s">
         <v>4</v>
       </c>
@@ -59649,11 +59596,8 @@
       <c r="G776">
         <v>0.70887234393788967</v>
       </c>
-      <c r="H776">
-        <v>5.8666666666666671</v>
-      </c>
-    </row>
-    <row r="777" spans="1:8">
+    </row>
+    <row r="777" spans="1:7">
       <c r="A777" t="s">
         <v>4</v>
       </c>
@@ -59672,11 +59616,8 @@
       <c r="G777">
         <v>1.6416455159382026</v>
       </c>
-      <c r="H777">
-        <v>13.2</v>
-      </c>
-    </row>
-    <row r="778" spans="1:8">
+    </row>
+    <row r="778" spans="1:7">
       <c r="A778" t="s">
         <v>4</v>
       </c>
@@ -59690,7 +59631,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="779" spans="1:8">
+    <row r="779" spans="1:7">
       <c r="A779" t="s">
         <v>4</v>
       </c>
@@ -59704,7 +59645,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="780" spans="1:8">
+    <row r="780" spans="1:7">
       <c r="A780" t="s">
         <v>4</v>
       </c>
@@ -59723,11 +59664,8 @@
       <c r="G780">
         <v>0.12990381056766589</v>
       </c>
-      <c r="H780">
-        <v>4.8499999999999996</v>
-      </c>
-    </row>
-    <row r="781" spans="1:8">
+    </row>
+    <row r="781" spans="1:7">
       <c r="A781" t="s">
         <v>4</v>
       </c>
@@ -59746,11 +59684,8 @@
       <c r="G781">
         <v>0.48653751140071555</v>
       </c>
-      <c r="H781">
-        <v>7.0749999999999993</v>
-      </c>
-    </row>
-    <row r="782" spans="1:8">
+    </row>
+    <row r="782" spans="1:7">
       <c r="A782" t="s">
         <v>4</v>
       </c>
@@ -59764,7 +59699,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="783" spans="1:8">
+    <row r="783" spans="1:7">
       <c r="A783" t="s">
         <v>4</v>
       </c>
@@ -59778,7 +59713,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="784" spans="1:8">
+    <row r="784" spans="1:7">
       <c r="A784" t="s">
         <v>4</v>
       </c>
@@ -59797,11 +59732,8 @@
       <c r="G784">
         <v>7.0710678118654655E-2</v>
       </c>
-      <c r="H784">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="785" spans="1:8">
+    </row>
+    <row r="785" spans="1:7">
       <c r="A785" t="s">
         <v>4</v>
       </c>
@@ -59820,11 +59752,8 @@
       <c r="G785">
         <v>1.0965856099730658</v>
       </c>
-      <c r="H785">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="786" spans="1:8">
+    </row>
+    <row r="786" spans="1:7">
       <c r="A786" t="s">
         <v>4</v>
       </c>
@@ -59843,11 +59772,8 @@
       <c r="G786">
         <v>1.1578664376775096</v>
       </c>
-      <c r="H786">
-        <v>10.797499999999999</v>
-      </c>
-    </row>
-    <row r="787" spans="1:8">
+    </row>
+    <row r="787" spans="1:7">
       <c r="A787" t="s">
         <v>4</v>
       </c>
@@ -59866,11 +59792,8 @@
       <c r="G787">
         <v>1.0280442597476069</v>
       </c>
-      <c r="H787">
-        <v>12.95</v>
-      </c>
-    </row>
-    <row r="788" spans="1:8">
+    </row>
+    <row r="788" spans="1:7">
       <c r="A788" t="s">
         <v>4</v>
       </c>
@@ -59889,11 +59812,8 @@
       <c r="G788">
         <v>0.42720018726587772</v>
       </c>
-      <c r="H788">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="789" spans="1:8">
+    </row>
+    <row r="789" spans="1:7">
       <c r="A789" t="s">
         <v>4</v>
       </c>
@@ -59912,11 +59832,8 @@
       <c r="G789">
         <v>0.25495097567963915</v>
       </c>
-      <c r="H789">
-        <v>7.8000000000000007</v>
-      </c>
-    </row>
-    <row r="790" spans="1:8">
+    </row>
+    <row r="790" spans="1:7">
       <c r="A790" t="s">
         <v>4</v>
       </c>
@@ -59935,11 +59852,8 @@
       <c r="G790">
         <v>1.1453711188955278</v>
       </c>
-      <c r="H790">
-        <v>10.350000000000001</v>
-      </c>
-    </row>
-    <row r="791" spans="1:8">
+    </row>
+    <row r="791" spans="1:7">
       <c r="A791" t="s">
         <v>4</v>
       </c>
@@ -59958,11 +59872,8 @@
       <c r="G791">
         <v>0.73950997288745202</v>
       </c>
-      <c r="H791">
-        <v>14.25</v>
-      </c>
-    </row>
-    <row r="792" spans="1:8">
+    </row>
+    <row r="792" spans="1:7">
       <c r="A792" t="s">
         <v>4</v>
       </c>
@@ -59981,11 +59892,8 @@
       <c r="G792">
         <v>0.42646805273080135</v>
       </c>
-      <c r="H792">
-        <v>6.85</v>
-      </c>
-    </row>
-    <row r="793" spans="1:8">
+    </row>
+    <row r="793" spans="1:7">
       <c r="A793" t="s">
         <v>4</v>
       </c>
@@ -60004,11 +59912,8 @@
       <c r="G793">
         <v>0.31917863337009256</v>
       </c>
-      <c r="H793">
-        <v>6.85</v>
-      </c>
-    </row>
-    <row r="794" spans="1:8">
+    </row>
+    <row r="794" spans="1:7">
       <c r="A794" t="s">
         <v>4</v>
       </c>
@@ -60027,11 +59932,8 @@
       <c r="G794">
         <v>1.3066392960568749</v>
       </c>
-      <c r="H794">
-        <v>10.734999999999999</v>
-      </c>
-    </row>
-    <row r="795" spans="1:8">
+    </row>
+    <row r="795" spans="1:7">
       <c r="A795" t="s">
         <v>4</v>
       </c>
@@ -60050,11 +59952,8 @@
       <c r="G795">
         <v>0.25495097567963931</v>
       </c>
-      <c r="H795">
-        <v>11.6</v>
-      </c>
-    </row>
-    <row r="796" spans="1:8">
+    </row>
+    <row r="796" spans="1:7">
       <c r="A796" t="s">
         <v>4</v>
       </c>
@@ -60073,11 +59972,8 @@
       <c r="G796">
         <v>0.26562295750848708</v>
       </c>
-      <c r="H796">
-        <v>6.3666666666666671</v>
-      </c>
-    </row>
-    <row r="797" spans="1:8">
+    </row>
+    <row r="797" spans="1:7">
       <c r="A797" t="s">
         <v>4</v>
       </c>
@@ -60096,11 +59992,8 @@
       <c r="G797">
         <v>4.330127018922178E-2</v>
       </c>
-      <c r="H797">
-        <v>6.5500000000000007</v>
-      </c>
-    </row>
-    <row r="798" spans="1:8">
+    </row>
+    <row r="798" spans="1:7">
       <c r="A798" t="s">
         <v>4</v>
       </c>
@@ -60119,11 +60012,8 @@
       <c r="G798">
         <v>1.1822991372744869</v>
       </c>
-      <c r="H798">
-        <v>9.5250000000000004</v>
-      </c>
-    </row>
-    <row r="799" spans="1:8">
+    </row>
+    <row r="799" spans="1:7">
       <c r="A799" t="s">
         <v>4</v>
       </c>
@@ -60142,11 +60032,8 @@
       <c r="G799">
         <v>1.1233320969330469</v>
       </c>
-      <c r="H799">
-        <v>11.25</v>
-      </c>
-    </row>
-    <row r="800" spans="1:8">
+    </row>
+    <row r="800" spans="1:7">
       <c r="A800" t="s">
         <v>4</v>
       </c>
@@ -60165,11 +60052,8 @@
       <c r="G800">
         <v>0.35000000000000009</v>
       </c>
-      <c r="H800">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="801" spans="1:8">
+    </row>
+    <row r="801" spans="1:7">
       <c r="A801" t="s">
         <v>4</v>
       </c>
@@ -60188,11 +60072,8 @@
       <c r="G801">
         <v>0.47631397208144094</v>
       </c>
-      <c r="H801">
-        <v>8.35</v>
-      </c>
-    </row>
-    <row r="802" spans="1:8">
+    </row>
+    <row r="802" spans="1:7">
       <c r="A802" t="s">
         <v>4</v>
       </c>
@@ -60211,11 +60092,8 @@
       <c r="G802">
         <v>0.5117372372614678</v>
       </c>
-      <c r="H802">
-        <v>11.549999999999999</v>
-      </c>
-    </row>
-    <row r="803" spans="1:8">
+    </row>
+    <row r="803" spans="1:7">
       <c r="A803" t="s">
         <v>4</v>
       </c>
@@ -60234,11 +60112,8 @@
       <c r="G803">
         <v>2.0425657884141697</v>
       </c>
-      <c r="H803">
-        <v>15.59</v>
-      </c>
-    </row>
-    <row r="804" spans="1:8">
+    </row>
+    <row r="804" spans="1:7">
       <c r="A804" t="s">
         <v>4</v>
       </c>
@@ -60257,11 +60132,8 @@
       <c r="G804">
         <v>0.3112474899497184</v>
       </c>
-      <c r="H804">
-        <v>6.4499999999999993</v>
-      </c>
-    </row>
-    <row r="805" spans="1:8">
+    </row>
+    <row r="805" spans="1:7">
       <c r="A805" t="s">
         <v>4</v>
       </c>
@@ -60280,11 +60152,8 @@
       <c r="G805">
         <v>0.2165063509461097</v>
       </c>
-      <c r="H805">
-        <v>6.65</v>
-      </c>
-    </row>
-    <row r="806" spans="1:8">
+    </row>
+    <row r="806" spans="1:7">
       <c r="A806" t="s">
         <v>4</v>
       </c>
@@ -60303,11 +60172,8 @@
       <c r="G806">
         <v>1.2852528934026968</v>
       </c>
-      <c r="H806">
-        <v>11.85</v>
-      </c>
-    </row>
-    <row r="807" spans="1:8">
+    </row>
+    <row r="807" spans="1:7">
       <c r="A807" t="s">
         <v>4</v>
       </c>
@@ -60326,11 +60192,8 @@
       <c r="G807">
         <v>1.7997829730275812</v>
       </c>
-      <c r="H807">
-        <v>12.324999999999999</v>
-      </c>
-    </row>
-    <row r="808" spans="1:8">
+    </row>
+    <row r="808" spans="1:7">
       <c r="A808" t="s">
         <v>4</v>
       </c>
@@ -60349,11 +60212,8 @@
       <c r="G808">
         <v>0.4023369234857751</v>
       </c>
-      <c r="H808">
-        <v>4.1500000000000004</v>
-      </c>
-    </row>
-    <row r="809" spans="1:8">
+    </row>
+    <row r="809" spans="1:7">
       <c r="A809" t="s">
         <v>4</v>
       </c>
@@ -60372,11 +60232,8 @@
       <c r="G809">
         <v>0.40311288741492768</v>
       </c>
-      <c r="H809">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="810" spans="1:8">
+    </row>
+    <row r="810" spans="1:7">
       <c r="A810" t="s">
         <v>4</v>
       </c>
@@ -60395,11 +60252,8 @@
       <c r="G810">
         <v>0.86998563206526625</v>
       </c>
-      <c r="H810">
-        <v>11.35</v>
-      </c>
-    </row>
-    <row r="811" spans="1:8">
+    </row>
+    <row r="811" spans="1:7">
       <c r="A811" t="s">
         <v>4</v>
       </c>
@@ -60418,11 +60272,8 @@
       <c r="G811">
         <v>0.59160797830996281</v>
       </c>
-      <c r="H811">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="812" spans="1:8">
+    </row>
+    <row r="812" spans="1:7">
       <c r="A812" t="s">
         <v>4</v>
       </c>
@@ -60441,11 +60292,8 @@
       <c r="G812">
         <v>0.2861380785564886</v>
       </c>
-      <c r="H812">
-        <v>4.95</v>
-      </c>
-    </row>
-    <row r="813" spans="1:8">
+    </row>
+    <row r="813" spans="1:7">
       <c r="A813" t="s">
         <v>4</v>
       </c>
@@ -60464,11 +60312,8 @@
       <c r="G813">
         <v>0.57608593109014572</v>
       </c>
-      <c r="H813">
-        <v>6.75</v>
-      </c>
-    </row>
-    <row r="814" spans="1:8">
+    </row>
+    <row r="814" spans="1:7">
       <c r="A814" t="s">
         <v>4</v>
       </c>
@@ -60487,11 +60332,8 @@
       <c r="G814">
         <v>1.6023420358962095</v>
       </c>
-      <c r="H814">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="815" spans="1:8">
+    </row>
+    <row r="815" spans="1:7">
       <c r="A815" t="s">
         <v>4</v>
       </c>
@@ -60510,11 +60352,8 @@
       <c r="G815">
         <v>1.5370807355178191</v>
       </c>
-      <c r="H815">
-        <v>14.8125</v>
-      </c>
-    </row>
-    <row r="816" spans="1:8">
+    </row>
+    <row r="816" spans="1:7">
       <c r="A816" t="s">
         <v>4</v>
       </c>
@@ -60533,11 +60372,8 @@
       <c r="G816">
         <v>0.18027756377320001</v>
       </c>
-      <c r="H816">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="817" spans="1:8">
+    </row>
+    <row r="817" spans="1:7">
       <c r="A817" t="s">
         <v>4</v>
       </c>
@@ -60556,11 +60392,8 @@
       <c r="G817">
         <v>0.25495097567963931</v>
       </c>
-      <c r="H817">
-        <v>8.2000000000000011</v>
-      </c>
-    </row>
-    <row r="818" spans="1:8">
+    </row>
+    <row r="818" spans="1:7">
       <c r="A818" t="s">
         <v>4</v>
       </c>
@@ -60579,11 +60412,8 @@
       <c r="G818">
         <v>0.54025456962435869</v>
       </c>
-      <c r="H818">
-        <v>10.35</v>
-      </c>
-    </row>
-    <row r="819" spans="1:8">
+    </row>
+    <row r="819" spans="1:7">
       <c r="A819" t="s">
         <v>4</v>
       </c>
@@ -60602,11 +60432,8 @@
       <c r="G819">
         <v>1.0520812706250384</v>
       </c>
-      <c r="H819">
-        <v>12.15</v>
-      </c>
-    </row>
-    <row r="820" spans="1:8">
+    </row>
+    <row r="820" spans="1:7">
       <c r="A820" t="s">
         <v>4</v>
       </c>
@@ -60625,11 +60452,8 @@
       <c r="G820">
         <v>0.38951091127207282</v>
       </c>
-      <c r="H820">
-        <v>3.7249999999999996</v>
-      </c>
-    </row>
-    <row r="821" spans="1:8">
+    </row>
+    <row r="821" spans="1:7">
       <c r="A821" t="s">
         <v>4</v>
       </c>
@@ -60648,11 +60472,8 @@
       <c r="G821">
         <v>0.43874821936960495</v>
       </c>
-      <c r="H821">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="822" spans="1:8">
+    </row>
+    <row r="822" spans="1:7">
       <c r="A822" t="s">
         <v>4</v>
       </c>
@@ -60671,11 +60492,8 @@
       <c r="G822">
         <v>0.37416573867739411</v>
       </c>
-      <c r="H822">
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="823" spans="1:8">
+    </row>
+    <row r="823" spans="1:7">
       <c r="A823" t="s">
         <v>4</v>
       </c>
@@ -60694,11 +60512,8 @@
       <c r="G823">
         <v>1.0825317547305451</v>
       </c>
-      <c r="H823">
-        <v>12.55</v>
-      </c>
-    </row>
-    <row r="824" spans="1:8">
+    </row>
+    <row r="824" spans="1:7">
       <c r="A824" t="s">
         <v>4</v>
       </c>
@@ -60717,11 +60532,8 @@
       <c r="G824">
         <v>0.20463381929681126</v>
       </c>
-      <c r="H824">
-        <v>5.15</v>
-      </c>
-    </row>
-    <row r="825" spans="1:8">
+    </row>
+    <row r="825" spans="1:7">
       <c r="A825" t="s">
         <v>4</v>
       </c>
@@ -60740,11 +60552,8 @@
       <c r="G825">
         <v>0.57268555944776545</v>
       </c>
-      <c r="H825">
-        <v>8.375</v>
-      </c>
-    </row>
-    <row r="826" spans="1:8">
+    </row>
+    <row r="826" spans="1:7">
       <c r="A826" t="s">
         <v>4</v>
       </c>
@@ -60763,11 +60572,8 @@
       <c r="G826">
         <v>0.80738776309775961</v>
       </c>
-      <c r="H826">
-        <v>12.95</v>
-      </c>
-    </row>
-    <row r="827" spans="1:8">
+    </row>
+    <row r="827" spans="1:7">
       <c r="A827" t="s">
         <v>4</v>
       </c>
@@ -60786,11 +60592,8 @@
       <c r="G827">
         <v>0.81729355191387199</v>
       </c>
-      <c r="H827">
-        <v>14.825000000000001</v>
-      </c>
-    </row>
-    <row r="828" spans="1:8">
+    </row>
+    <row r="828" spans="1:7">
       <c r="A828" t="s">
         <v>4</v>
       </c>
@@ -60809,11 +60612,8 @@
       <c r="G828">
         <v>0.12247448713915901</v>
       </c>
-      <c r="H828">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="829" spans="1:8">
+    </row>
+    <row r="829" spans="1:7">
       <c r="A829" t="s">
         <v>4</v>
       </c>
@@ -60832,11 +60632,8 @@
       <c r="G829">
         <v>1.0606601717798247</v>
       </c>
-      <c r="H829">
-        <v>11.8</v>
-      </c>
-    </row>
-    <row r="830" spans="1:8">
+    </row>
+    <row r="830" spans="1:7">
       <c r="A830" t="s">
         <v>4</v>
       </c>
@@ -60855,11 +60652,8 @@
       <c r="G830">
         <v>0.36314597615834865</v>
       </c>
-      <c r="H830">
-        <v>13.05</v>
-      </c>
-    </row>
-    <row r="831" spans="1:8">
+    </row>
+    <row r="831" spans="1:7">
       <c r="A831" t="s">
         <v>4</v>
       </c>
@@ -60877,9 +60671,6 @@
       </c>
       <c r="G831">
         <v>1.6618889854620265</v>
-      </c>
-      <c r="H831">
-        <v>13.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed errors in observed files for new POStats
</commit_message>
<xml_diff>
--- a/Tests/Validation/Mungbean/ObservedData.xlsx
+++ b/Tests/Validation/Mungbean/ObservedData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ApsimX\Tests\Validation\Mungbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98976905-E26D-4E1D-941A-CDEDCD224005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B01E149-1D03-4811-BD5E-37D3CAE2ED6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{9FA297CA-29B6-4A83-B4E5-4BA784BC781A}"/>
   </bookViews>
@@ -1140,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D7DBC0-8FFD-4004-98F0-2F6AD6B427E8}">
   <dimension ref="A1:W442"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView topLeftCell="A146" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -11690,7 +11690,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12219,9 +12219,6 @@
       </c>
       <c r="E25">
         <v>12.58</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
       </c>
       <c r="H25">
         <v>4.7400000000000005E-2</v>

</xml_diff>